<commit_message>
testy pso dla PID i NPL skonczone
</commit_message>
<xml_diff>
--- a/tabelki/tabelki.xlsx
+++ b/tabelki/tabelki.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1c0a2aad9fadc03e/Documents/GitHub/SZAU_3/tabelki/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="65" documentId="8_{4DADEFDA-A948-4255-A03D-4EBC032A3321}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{96956A02-3AEF-400E-8E5D-DD98C097B40B}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{4DADEFDA-A948-4255-A03D-4EBC032A3321}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{DAF066FB-725F-4512-961B-985984D5A23E}"/>
   <bookViews>
-    <workbookView xWindow="2424" yWindow="624" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{2E4A838C-DFE1-4C9D-BCB1-239EC32A0C63}"/>
+    <workbookView xWindow="2424" yWindow="624" windowWidth="17280" windowHeight="8964" activeTab="5" xr2:uid="{2E4A838C-DFE1-4C9D-BCB1-239EC32A0C63}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
-    <sheet name="NPL_C2" sheetId="6" r:id="rId2"/>
-    <sheet name="NPL_C1" sheetId="5" r:id="rId3"/>
-    <sheet name="PID_C1" sheetId="2" r:id="rId4"/>
-    <sheet name="PID_C2" sheetId="3" r:id="rId5"/>
-    <sheet name="PID_pop" sheetId="4" r:id="rId6"/>
+    <sheet name="Arkusz3" sheetId="8" r:id="rId2"/>
+    <sheet name="NPL_all" sheetId="7" r:id="rId3"/>
+    <sheet name="NPL_C2" sheetId="6" r:id="rId4"/>
+    <sheet name="NPL_C1" sheetId="5" r:id="rId5"/>
+    <sheet name="PID_C1" sheetId="2" r:id="rId6"/>
+    <sheet name="PID_C2" sheetId="3" r:id="rId7"/>
+    <sheet name="PID_pop" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="203">
   <si>
     <t>'PID'</t>
   </si>
@@ -615,6 +617,39 @@
   </si>
   <si>
     <t>lambda</t>
+  </si>
+  <si>
+    <t>38.0799899810620</t>
+  </si>
+  <si>
+    <t>0.897379841180761</t>
+  </si>
+  <si>
+    <t>wartości domyślne</t>
+  </si>
+  <si>
+    <t>zmienne C1</t>
+  </si>
+  <si>
+    <t>zmienne C2</t>
+  </si>
+  <si>
+    <t>zmienna populacja</t>
+  </si>
+  <si>
+    <t>małe wartości parametrów</t>
+  </si>
+  <si>
+    <t>duże wartości parametrów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PID best </t>
+  </si>
+  <si>
+    <t>NPL best</t>
+  </si>
+  <si>
+    <t>PID best</t>
   </si>
 </sst>
 </file>
@@ -631,7 +666,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -644,8 +679,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -783,11 +824,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -826,6 +925,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -1140,10 +1267,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C923FA-B8C3-45E2-B02A-A1B0A899B25C}">
-  <dimension ref="B2:V55"/>
+  <dimension ref="B2:V56"/>
   <sheetViews>
-    <sheetView topLeftCell="B40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47:J52"/>
+    <sheetView topLeftCell="G37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42:U42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1152,7 +1279,7 @@
     <col min="18" max="18" width="13.6640625" customWidth="1"/>
     <col min="19" max="19" width="14.109375" customWidth="1"/>
     <col min="20" max="20" width="5.44140625" customWidth="1"/>
-    <col min="21" max="21" width="5.21875" customWidth="1"/>
+    <col min="21" max="21" width="10.33203125" customWidth="1"/>
     <col min="22" max="22" width="9" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3201,6 +3328,9 @@
       <c r="J40">
         <v>40</v>
       </c>
+      <c r="O40" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="41" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B41">
@@ -3259,6 +3389,27 @@
       <c r="J42">
         <v>40</v>
       </c>
+      <c r="O42" t="s">
+        <v>1</v>
+      </c>
+      <c r="P42" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>114</v>
+      </c>
+      <c r="R42" t="s">
+        <v>115</v>
+      </c>
+      <c r="S42" t="s">
+        <v>5</v>
+      </c>
+      <c r="T42" t="s">
+        <v>6</v>
+      </c>
+      <c r="U42">
+        <v>100</v>
+      </c>
     </row>
     <row r="43" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B43">
@@ -3346,8 +3497,11 @@
       <c r="J45">
         <v>40</v>
       </c>
-    </row>
-    <row r="46" spans="2:22" x14ac:dyDescent="0.3">
+      <c r="O45" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="46" spans="2:22" ht="36" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46">
         <v>44</v>
       </c>
@@ -3374,6 +3528,27 @@
       </c>
       <c r="J46">
         <v>40</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="P46" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q46" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="R46" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="S46" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="T46" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="U46" s="5" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="47" spans="2:22" x14ac:dyDescent="0.3">
@@ -3404,6 +3579,27 @@
       <c r="J47">
         <v>10</v>
       </c>
+      <c r="O47" s="3">
+        <v>37.924627387027797</v>
+      </c>
+      <c r="P47" s="3">
+        <v>20</v>
+      </c>
+      <c r="Q47" s="3">
+        <v>21</v>
+      </c>
+      <c r="R47" s="3">
+        <v>0.78830418173989103</v>
+      </c>
+      <c r="S47" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="T47" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="U47" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="48" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B48">
@@ -3635,6 +3831,35 @@
       </c>
       <c r="J55">
         <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>54</v>
+      </c>
+      <c r="C56" t="s">
+        <v>142</v>
+      </c>
+      <c r="D56" t="s">
+        <v>192</v>
+      </c>
+      <c r="E56">
+        <v>27</v>
+      </c>
+      <c r="F56">
+        <v>14</v>
+      </c>
+      <c r="G56" t="s">
+        <v>193</v>
+      </c>
+      <c r="H56" t="s">
+        <v>132</v>
+      </c>
+      <c r="I56" t="s">
+        <v>133</v>
+      </c>
+      <c r="J56">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -3644,11 +3869,776 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3135B0BE-B9A4-4611-AEB0-5E9CDB9398FB}">
+  <dimension ref="A4:E38"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="14.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="C4" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="24" t="s">
+        <v>194</v>
+      </c>
+      <c r="B5" s="24"/>
+      <c r="C5" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="E5" s="25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="27">
+        <v>1.25</v>
+      </c>
+      <c r="E6" s="27">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="28"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="25">
+        <v>2.5</v>
+      </c>
+      <c r="D7" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="E7" s="25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="27">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="27">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="22"/>
+      <c r="B9" s="22"/>
+      <c r="C9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="25">
+        <v>2.5</v>
+      </c>
+      <c r="E10" s="25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="26"/>
+      <c r="C11" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="27">
+        <v>1.25</v>
+      </c>
+      <c r="E11" s="27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="25">
+        <v>0.5</v>
+      </c>
+      <c r="D12" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="E12" s="25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="30" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="30"/>
+      <c r="C13" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="D13" s="31">
+        <v>0.2</v>
+      </c>
+      <c r="E13" s="31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>198</v>
+      </c>
+      <c r="B14" s="29"/>
+      <c r="C14" s="23">
+        <v>1.6</v>
+      </c>
+      <c r="D14" s="23">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E14" s="23">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C17">
+        <v>0.5</v>
+      </c>
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+      <c r="E17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C18">
+        <v>0.5</v>
+      </c>
+      <c r="D18">
+        <v>0.1</v>
+      </c>
+      <c r="E18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C19">
+        <v>0.5</v>
+      </c>
+      <c r="D19">
+        <v>0.1</v>
+      </c>
+      <c r="E19">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C20">
+        <v>0.5</v>
+      </c>
+      <c r="D20">
+        <v>0.6</v>
+      </c>
+      <c r="E20">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C21">
+        <v>0.5</v>
+      </c>
+      <c r="D21">
+        <v>0.5</v>
+      </c>
+      <c r="E21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C22">
+        <v>0.5</v>
+      </c>
+      <c r="D22">
+        <v>0.5</v>
+      </c>
+      <c r="E22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C23">
+        <v>0.5</v>
+      </c>
+      <c r="D23">
+        <v>0.5</v>
+      </c>
+      <c r="E23">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C24">
+        <v>0.5</v>
+      </c>
+      <c r="D24">
+        <v>2.5</v>
+      </c>
+      <c r="E24">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C25">
+        <v>0.5</v>
+      </c>
+      <c r="D25">
+        <v>2.5</v>
+      </c>
+      <c r="E25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C26">
+        <v>0.5</v>
+      </c>
+      <c r="D26">
+        <v>2.5</v>
+      </c>
+      <c r="E26">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="27" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C27">
+        <v>0.5</v>
+      </c>
+      <c r="D27">
+        <v>1.25</v>
+      </c>
+      <c r="E27">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C28">
+        <v>0.5</v>
+      </c>
+      <c r="D28">
+        <v>1.25</v>
+      </c>
+      <c r="E28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C29">
+        <v>0.5</v>
+      </c>
+      <c r="D29">
+        <v>1.25</v>
+      </c>
+      <c r="E29">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C30">
+        <v>0.5</v>
+      </c>
+      <c r="D30">
+        <v>1.25</v>
+      </c>
+      <c r="E30">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C31">
+        <v>0.5</v>
+      </c>
+      <c r="D31">
+        <v>1.25</v>
+      </c>
+      <c r="E31">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C32">
+        <v>0.5</v>
+      </c>
+      <c r="D32">
+        <v>1.25</v>
+      </c>
+      <c r="E32">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C33">
+        <v>0.2</v>
+      </c>
+      <c r="D33">
+        <v>0.2</v>
+      </c>
+      <c r="E33">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C34">
+        <v>0.2</v>
+      </c>
+      <c r="D34">
+        <v>0.2</v>
+      </c>
+      <c r="E34">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C35">
+        <v>0.2</v>
+      </c>
+      <c r="D35">
+        <v>0.2</v>
+      </c>
+      <c r="E35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="36" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C36">
+        <v>1.6</v>
+      </c>
+      <c r="D36">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C37">
+        <v>1.6</v>
+      </c>
+      <c r="D37">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E37">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C38">
+        <v>1.6</v>
+      </c>
+      <c r="D38">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="E38">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A6:B7"/>
+    <mergeCell ref="A8:B10"/>
+    <mergeCell ref="A11:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9AFBF17-C327-429F-BB42-537901464D01}">
+  <dimension ref="B4:H23"/>
+  <sheetViews>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="3">
+        <v>38.081054343597202</v>
+      </c>
+      <c r="C5" s="3">
+        <v>17</v>
+      </c>
+      <c r="D5" s="3">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.80237308671172602</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="3">
+        <v>39.001035684195998</v>
+      </c>
+      <c r="C6" s="3">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3">
+        <v>10</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.80615048265364697</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H6" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="3">
+        <v>38.966741021850297</v>
+      </c>
+      <c r="C7" s="3">
+        <v>12</v>
+      </c>
+      <c r="D7" s="3">
+        <v>5</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.81721463226930502</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="3">
+        <v>38.079989981061999</v>
+      </c>
+      <c r="C8" s="3">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3">
+        <v>14</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.89737984118076097</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="G8" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H8" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B10" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="3">
+        <v>74.752494564765499</v>
+      </c>
+      <c r="C11" s="3">
+        <v>-9.0228068784291293E-2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1.9221275101611699</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.38157051048178398</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="3">
+        <v>70.6712612270031</v>
+      </c>
+      <c r="C12" s="3">
+        <v>-0.11845329306708099</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2.4527138745745201</v>
+      </c>
+      <c r="E12" s="3">
+        <v>1.0409428310075601E-2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H12" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="3">
+        <v>82.235502243203996</v>
+      </c>
+      <c r="C13" s="3">
+        <v>-5.9332461679248397E-2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>1.23890369661688</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.2259742772518</v>
+      </c>
+      <c r="F13" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="H13" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="3">
+        <v>40.728586743218997</v>
+      </c>
+      <c r="C14" s="3">
+        <v>-0.65963944155994703</v>
+      </c>
+      <c r="D14" s="3">
+        <v>12.131483700736799</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.42274041090005698</v>
+      </c>
+      <c r="F14" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="G14" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H14" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="3">
+        <v>40.728586715431099</v>
+      </c>
+      <c r="C15" s="3">
+        <v>-0.65961970576123097</v>
+      </c>
+      <c r="D15" s="3">
+        <v>12.128688295102901</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.42285802824630297</v>
+      </c>
+      <c r="F15" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="G15" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H15" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="3">
+        <v>40.728586764185401</v>
+      </c>
+      <c r="C16" s="3">
+        <v>-0.65962965917927796</v>
+      </c>
+      <c r="D16" s="3">
+        <v>12.1317219831753</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.42261401365882101</v>
+      </c>
+      <c r="F16" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="G16" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H16" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B22" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="3">
+        <v>37.924627387027797</v>
+      </c>
+      <c r="C23" s="3">
+        <v>20</v>
+      </c>
+      <c r="D23" s="3">
+        <v>21</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.78830418173989103</v>
+      </c>
+      <c r="F23" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G23" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="H23" s="3">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE1517D4-409E-46B9-BCAC-76D8A8BD5E09}">
   <dimension ref="B4:H17"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3923,12 +4913,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A04D2E3-EC6C-4199-84CF-436871299153}">
   <dimension ref="B4:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:E4"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4147,12 +5137,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{573F7BEA-E6BF-48CF-B693-BC80DCCA8823}">
-  <dimension ref="B2:H19"/>
+  <dimension ref="B2:H26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4457,13 +5447,64 @@
         <v>40</v>
       </c>
     </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B25" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B26" s="3">
+        <v>40.728586612188202</v>
+      </c>
+      <c r="C26" s="3">
+        <v>-0.65963247405484304</v>
+      </c>
+      <c r="D26" s="3">
+        <v>12.130246687725601</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.42274256133532301</v>
+      </c>
+      <c r="F26" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G26" s="3">
+        <v>1.25</v>
+      </c>
+      <c r="H26" s="3">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D49B9C5F-9972-487F-B079-00ECF1D3E3D1}">
   <dimension ref="B2:H12"/>
   <sheetViews>
@@ -4713,12 +5754,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56DCAD2F-97E2-41C7-84EE-291D71592161}">
   <dimension ref="B3:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:H10"/>
+      <selection activeCell="F3" sqref="F3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>